<commit_message>
update doc, fix comment
</commit_message>
<xml_diff>
--- a/doc/book_templates解析.xlsx
+++ b/doc/book_templates解析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user1\work\workspace\git\bookproject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6FB574-C8BB-439D-B2BD-1D877B724F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA4FA06-F37C-4BFB-B12F-1F2B18FCF5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="607" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="607" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index.html" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="207">
   <si>
     <r>
       <t xml:space="preserve">{% </t>
@@ -6547,146 +6547,6 @@
         <family val="3"/>
       </rPr>
       <t>{% comment %} Bookオブジェクト送信用 {% endcomment %}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF808080"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"hidden"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"book"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"{{ book.id }}"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF808080"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
     </r>
   </si>
   <si>
@@ -9035,6 +8895,283 @@
     <t>↑(ここはセキュリティ対策)</t>
     <rPh sb="11" eb="13">
       <t>タイサク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>継承元定義</t>
+    <rPh sb="0" eb="3">
+      <t>ケイショウモト</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>テイギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メソッドにpostを指定</t>
+    <rPh sb="10" eb="12">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>formに画像を含むための処理</t>
+    <rPh sb="5" eb="7">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ショリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UpdateBookViewで指定したfieldを表示</t>
+    <rPh sb="15" eb="17">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ベースの継承</t>
+    <rPh sb="4" eb="6">
+      <t>ケイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>基底クラスのコンテンツ</t>
+    <rPh sb="0" eb="2">
+      <t>キテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>postメソッド</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ラベル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入力フォーム</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>選択式の入力フォーム</t>
+    <rPh sb="0" eb="2">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>シキ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入力フォーム, bookはviewからレンダリング時に渡してるから使える。</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ワタ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿ボタン</t>
+    <rPh sb="0" eb="2">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"hidden"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"book"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"{{ book.id }}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">フォームでどのbookかを指定する必要がある。
+しかしviewを開いている時点でどのbookかは決まっているので、ユーザーに選ばせたくない。
+そのためhiddenで表示せずにpostメソッドで送信している。
+</t>
+    <rPh sb="13" eb="15">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ジテン</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>ソウシン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -9120,7 +9257,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9139,6 +9276,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -9152,7 +9295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9168,6 +9311,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -9650,6 +9794,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>10675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38870</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16045C69-DD99-025A-2A99-BDF7C2A44CEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687425" y="2857500"/>
+          <a:ext cx="8240275" cy="5515745"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>363092</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>191413</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{971BCFF5-F074-C77D-07BB-E7F2239A8C79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14097000" y="8648700"/>
+          <a:ext cx="8183117" cy="6544588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9925,16 +10162,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -9942,10 +10179,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9953,10 +10190,10 @@
         <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -9964,10 +10201,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -9975,10 +10212,10 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -9986,10 +10223,10 @@
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -9997,10 +10234,10 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -10008,10 +10245,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="93.75">
@@ -10019,10 +10256,10 @@
         <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -10030,21 +10267,21 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
         <v>124</v>
       </c>
-      <c r="C11" t="s">
-        <v>125</v>
-      </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -10052,10 +10289,10 @@
         <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -10063,10 +10300,10 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -10074,21 +10311,21 @@
         <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
         <v>130</v>
       </c>
-      <c r="C15" t="s">
-        <v>131</v>
-      </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -10096,10 +10333,10 @@
         <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -10107,10 +10344,10 @@
         <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -10118,10 +10355,10 @@
         <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -10129,10 +10366,10 @@
         <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -10140,10 +10377,10 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -10151,10 +10388,10 @@
         <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -10162,10 +10399,10 @@
         <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -10173,10 +10410,10 @@
         <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -10184,10 +10421,10 @@
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -10195,21 +10432,21 @@
         <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="168.75">
       <c r="B26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="D26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -10217,10 +10454,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -10228,10 +10465,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -10239,10 +10476,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -10250,10 +10487,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -10261,10 +10498,10 @@
         <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -10272,10 +10509,10 @@
         <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -10283,10 +10520,10 @@
         <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -10294,10 +10531,10 @@
         <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -10305,10 +10542,10 @@
         <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -10316,10 +10553,10 @@
         <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -10327,10 +10564,10 @@
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -10338,10 +10575,10 @@
         <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -10349,10 +10586,10 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -10360,10 +10597,10 @@
         <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -10371,10 +10608,10 @@
         <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -10382,10 +10619,10 @@
         <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -10393,10 +10630,10 @@
         <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -10404,10 +10641,10 @@
         <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -10415,10 +10652,10 @@
         <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -10426,10 +10663,10 @@
         <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -10437,10 +10674,10 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -10448,10 +10685,10 @@
         <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -10459,10 +10696,10 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -10470,10 +10707,10 @@
         <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -10481,10 +10718,10 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -10492,10 +10729,10 @@
         <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -10503,10 +10740,10 @@
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -10530,16 +10767,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -10547,10 +10784,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -10558,10 +10795,10 @@
         <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -10569,10 +10806,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -10580,10 +10817,10 @@
         <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -10591,10 +10828,10 @@
         <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -10602,10 +10839,10 @@
         <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -10613,21 +10850,21 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="37.5">
       <c r="B9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -10635,10 +10872,10 @@
         <v>42</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -10646,10 +10883,10 @@
         <v>43</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -10657,10 +10894,10 @@
         <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -10668,10 +10905,10 @@
         <v>45</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="37.5">
@@ -10679,10 +10916,10 @@
         <v>46</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -10690,10 +10927,10 @@
         <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -10701,10 +10938,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -10712,10 +10949,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -10723,10 +10960,10 @@
         <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -10734,10 +10971,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -10760,16 +10997,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -10777,10 +11014,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -10788,10 +11025,10 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -10799,10 +11036,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -10810,10 +11047,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -10821,10 +11058,10 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -10832,10 +11069,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -10843,10 +11080,10 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -10854,10 +11091,10 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -10865,21 +11102,21 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="93.75">
       <c r="B11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>161</v>
-      </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -10887,10 +11124,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -10898,10 +11135,10 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -10909,10 +11146,10 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -10920,10 +11157,10 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -10931,10 +11168,10 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -10942,10 +11179,10 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -10953,10 +11190,10 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -10964,10 +11201,10 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -10975,10 +11212,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -10986,10 +11223,10 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -10997,10 +11234,10 @@
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -11008,10 +11245,10 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -11019,10 +11256,10 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -11030,10 +11267,10 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -11041,10 +11278,10 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -11052,10 +11289,10 @@
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -11063,10 +11300,10 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -11074,10 +11311,10 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -11102,17 +11339,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>118</v>
+      <c r="A1" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -11120,10 +11357,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11131,10 +11368,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11142,10 +11379,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -11153,10 +11390,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11164,24 +11401,24 @@
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="202.5">
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -11189,10 +11426,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11200,21 +11437,21 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="150">
       <c r="B10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11222,10 +11459,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11233,10 +11470,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11244,10 +11481,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -11261,7 +11498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B13612-F4A7-428E-B5C3-349FF179BC07}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -11271,20 +11508,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>118</v>
+      <c r="A1" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -11292,13 +11529,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -11306,10 +11543,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -11317,13 +11554,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -11331,10 +11568,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
@@ -11345,13 +11582,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -11359,10 +11596,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -11370,13 +11607,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -11384,13 +11621,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -11398,50 +11635,50 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="G11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="G12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="G13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="G14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="G15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="G16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="7:7">
       <c r="G17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="7:7">
       <c r="G18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -11452,78 +11689,124 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F33F50-928B-4AF8-9253-E1C1E776C752}">
-  <dimension ref="B1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="2" max="2" width="107.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:2">
+      <c r="C1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:2">
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="2:2">
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="C5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:2">
+      <c r="C6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="2:2">
+      <c r="C7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:2">
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:2">
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="2:2">
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="2:2">
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:2">
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -11534,173 +11817,366 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685755CE-0B02-42A8-B857-331C5C962125}">
-  <dimension ref="B1:B31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="2" max="2" width="107.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:2">
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:2">
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="2:2">
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="2:2">
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="2:2">
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:2">
+      <c r="C8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:2">
+      <c r="C9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:2">
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:2">
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="2:2">
+      <c r="C12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="2:2">
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="2:2">
+      <c r="C14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="2:2">
+      <c r="C15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="2:2">
+      <c r="C16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="2:2">
+      <c r="C17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="2:2">
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="2:2">
+      <c r="C19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="2:2">
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
       <c r="B21" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="2:2">
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
       <c r="B22" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="2:2">
+      <c r="C22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
       <c r="B23" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="2:2">
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
       <c r="B24" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
       <c r="B25" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="2:2">
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
       <c r="B26" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" spans="2:2">
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="2:2">
+      <c r="C27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="131.25">
       <c r="B28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
+      <c r="C29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="2:2">
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
       <c r="B31" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11708,7 +12184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EA06B3-54C3-4FDD-B7D8-2F1F4111270E}">
   <dimension ref="B1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -11718,107 +12194,107 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>